<commit_message>
- fixed EXCEL.clear where it was missing last column - skip pause when running nexial under JUnit
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_expressions.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_expressions.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F113A46-EAF9-2F4A-B4D0-52C064ECDA5C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A58019-0479-7B4D-B70D-2874D17DCA2F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="440" windowWidth="33600" windowHeight="12540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27320" yWindow="440" windowWidth="13640" windowHeight="12580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -920,7 +920,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
- add more tests - organize test code a bit to reduce LOC
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_expressions.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_expressions.data.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FAF850-256D-0D42-991B-0A0446A76304}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BFEF25-4688-7F4C-B26B-831D739EABC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="20480" windowHeight="12580" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
-    <sheet name="NUMBER" sheetId="3" r:id="rId2"/>
-    <sheet name="EXCEL" sheetId="4" r:id="rId3"/>
-    <sheet name="XML" sheetId="5" r:id="rId4"/>
+    <sheet name="EXCEL" sheetId="4" r:id="rId2"/>
+    <sheet name="XML" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -234,72 +233,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -786,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -864,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
@@ -884,21 +818,21 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="19" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -908,87 +842,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EAA04C-BF70-B242-9A9B-10C3884AAE5A}">
-  <dimension ref="A1:AAA10"/>
-  <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="209:703">
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="209:703">
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="209:703">
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="209:703">
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="209:703">
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="209:703">
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="209:703">
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="209:703">
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="209:703">
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="209:703">
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9FF33A-0786-5841-812D-9BBD01196397}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
@@ -1077,11 +930,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254055EB-DCB9-524E-8590-28E4C5156F9C}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>